<commit_message>
- Change lib gopdf by my fork
</commit_message>
<xml_diff>
--- a/demo/result.xlsx
+++ b/demo/result.xlsx
@@ -129,22 +129,22 @@
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" applyProtection="0" borderId="2" fillId="3" fontId="2" numFmtId="49">
-      <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="3" fontId="2" numFmtId="0">
-      <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="3" fontId="3" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="0"/>
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" applyProtection="0" borderId="4" fillId="3" fontId="3" numFmtId="49">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="0"/>
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="1" applyProtection="0" borderId="4" fillId="3" fontId="0" numFmtId="49">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="0"/>
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" applyFont="1" applyFill="1" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="3" fontId="0" numFmtId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="0"/>
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
 </styleSheet>

</xml_diff>